<commit_message>
funcionando adição de todos os dados na planilha
</commit_message>
<xml_diff>
--- a/php/result.xlsx
+++ b/php/result.xlsx
@@ -249,7 +249,7 @@
         </is>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:11">
       <c r="A2" s="0" t="inlineStr">
         <is>
           <t>137458</t>
@@ -265,8 +265,48 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="0" t="inlineStr">
+        <is>
+          <t>Bryan Nickson Santana Pinto;</t>
+        </is>
+      </c>
+      <c r="E2" s="0" t="inlineStr">
+        <is>
+          <t>Departamento de Química / Centro de Ciências Exatas e Tecnológicas / Universidade Federal de Viçosa - Campus Viçosa</t>
+        </is>
+      </c>
+      <c r="F2" s="0" t="inlineStr">
+        <is>
+          <t>Gabriella Almeida  Moura;</t>
+        </is>
+      </c>
+      <c r="G2" s="0" t="inlineStr">
+        <is>
+          <t>Departamento de Química / Centro de Ciências Exatas e Tecnológicas / Universidade Federal de Viçosa - Campus Viçosa</t>
+        </is>
+      </c>
+      <c r="H2" s="0" t="inlineStr">
+        <is>
+          <t>Antonio Demuner;</t>
+        </is>
+      </c>
+      <c r="I2" s="0" t="inlineStr">
+        <is>
+          <t>Departamento de Química / Centro de Ciências Exatas e Tecnológicas / Universidade Federal de Viçosa - Campus Viçosa</t>
+        </is>
+      </c>
+      <c r="J2" s="0" t="inlineStr">
+        <is>
+          <t>Elson Santiago Alvarenga;</t>
+        </is>
+      </c>
+      <c r="K2" s="0" t="inlineStr">
+        <is>
+          <t>Departamento de Química / Centro de Ciências Exatas e Tecnológicas / Universidade Federal de Viçosa - Campus Viçosa</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="0" t="inlineStr">
         <is>
           <t>137459</t>
@@ -282,8 +322,18 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>Tiago   Bueno de Moraes;</t>
+        </is>
+      </c>
+      <c r="E3" s="0" t="inlineStr">
+        <is>
+          <t>Departamento de Química  / Instituto de Ciências Exatas  / Universidade Federal de Minas Gerais</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="0" t="inlineStr">
         <is>
           <t>137460</t>
@@ -299,8 +349,38 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>Tatiana Monaretto;</t>
+        </is>
+      </c>
+      <c r="E4" s="0" t="inlineStr">
+        <is>
+          <t>Centre national de la recherche scientifique (CNRS)</t>
+        </is>
+      </c>
+      <c r="F4" s="0" t="inlineStr">
+        <is>
+          <t>Luiz Alberto Colnago;</t>
+        </is>
+      </c>
+      <c r="G4" s="0" t="inlineStr">
+        <is>
+          <t>Empresa Brasileira de Pesquisa Agropecuária</t>
+        </is>
+      </c>
+      <c r="H4" s="0" t="inlineStr">
+        <is>
+          <t>Tiago   Bueno de Moraes;</t>
+        </is>
+      </c>
+      <c r="I4" s="0" t="inlineStr">
+        <is>
+          <t>Departamento de Química  / Instituto de Ciências Exatas  / Universidade Federal de Minas Gerais</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" spans="1:35">
       <c r="A5" s="0" t="inlineStr">
         <is>
           <t>137464</t>
@@ -316,8 +396,168 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>Katelyn Downey;</t>
+        </is>
+      </c>
+      <c r="E5" s="0" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Sciences / Environmental NMR Centre / University of Toronto</t>
+        </is>
+      </c>
+      <c r="F5" s="0" t="inlineStr">
+        <is>
+          <t>Bing Wu;</t>
+        </is>
+      </c>
+      <c r="G5" s="0" t="inlineStr">
+        <is>
+          <t>Environmental NMR Centre / University of Toronto</t>
+        </is>
+      </c>
+      <c r="H5" s="0" t="inlineStr">
+        <is>
+          <t>Rudraksha Majumdar;</t>
+        </is>
+      </c>
+      <c r="I5" s="0" t="inlineStr">
+        <is>
+          <t>Synex Medical</t>
+        </is>
+      </c>
+      <c r="J5" s="0" t="inlineStr">
+        <is>
+          <t>Daniel Lysak;</t>
+        </is>
+      </c>
+      <c r="K5" s="0" t="inlineStr">
+        <is>
+          <t>Chemistry / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
+      <c r="L5" s="0" t="inlineStr">
+        <is>
+          <t>Rajshree Ghosh Biswas;</t>
+        </is>
+      </c>
+      <c r="M5" s="0" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
+      <c r="N5" s="0" t="inlineStr">
+        <is>
+          <t>Maryam  Tabatabaei-Anaraki;</t>
+        </is>
+      </c>
+      <c r="O5" s="0" t="inlineStr">
+        <is>
+          <t>Chemistry / Environmental NMR Centre / University of Toronto</t>
+        </is>
+      </c>
+      <c r="P5" s="0" t="inlineStr">
+        <is>
+          <t>Amy Jenne;</t>
+        </is>
+      </c>
+      <c r="Q5" s="0" t="inlineStr">
+        <is>
+          <t>Chemistry / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
+      <c r="R5" s="0" t="inlineStr">
+        <is>
+          <t>Xiang You;</t>
+        </is>
+      </c>
+      <c r="S5" s="0" t="inlineStr">
+        <is>
+          <t>Environmental NMR Centre / University of Toronto</t>
+        </is>
+      </c>
+      <c r="T5" s="0" t="inlineStr">
+        <is>
+          <t>Ronald Soong;</t>
+        </is>
+      </c>
+      <c r="U5" s="0" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
+      <c r="V5" s="0" t="inlineStr">
+        <is>
+          <t>Daniel Lane;</t>
+        </is>
+      </c>
+      <c r="W5" s="0" t="inlineStr">
+        <is>
+          <t>Environmental NMR Centre / University of Toronto</t>
+        </is>
+      </c>
+      <c r="X5" s="0" t="inlineStr">
+        <is>
+          <t>Paul Helm;</t>
+        </is>
+      </c>
+      <c r="Y5" s="0" t="inlineStr">
+        <is>
+          <t>Environmental Monitoring &amp; Reporting Branch / Ontario Ministry of the Environment</t>
+        </is>
+      </c>
+      <c r="Z5" s="0" t="inlineStr">
+        <is>
+          <t>Anna Codina;</t>
+        </is>
+      </c>
+      <c r="AA5" s="0" t="inlineStr">
+        <is>
+          <t>Bruker</t>
+        </is>
+      </c>
+      <c r="AB5" s="0" t="inlineStr">
+        <is>
+          <t>Venita Decker;</t>
+        </is>
+      </c>
+      <c r="AC5" s="0" t="inlineStr">
+        <is>
+          <t>Bruker</t>
+        </is>
+      </c>
+      <c r="AD5" s="0" t="inlineStr">
+        <is>
+          <t>Falko Busse;</t>
+        </is>
+      </c>
+      <c r="AE5" s="0" t="inlineStr">
+        <is>
+          <t>Bruker</t>
+        </is>
+      </c>
+      <c r="AF5" s="0" t="inlineStr">
+        <is>
+          <t>Myrna Simpson;</t>
+        </is>
+      </c>
+      <c r="AG5" s="0" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Sciences / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
+      <c r="AH5" s="0" t="inlineStr">
+        <is>
+          <t>Andre Simpson;</t>
+        </is>
+      </c>
+      <c r="AI5" s="0" t="inlineStr">
+        <is>
+          <t>University of Toronto</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="0" t="inlineStr">
         <is>
           <t>137465</t>
@@ -333,8 +573,58 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>Banny S. B. Correia;</t>
+        </is>
+      </c>
+      <c r="E6" s="0" t="inlineStr">
+        <is>
+          <t>Instituto de Química de São Carlos  / Universidade de São Paulo</t>
+        </is>
+      </c>
+      <c r="F6" s="0" t="inlineStr">
+        <is>
+          <t>Pollyana Ferreira da Silva Vianna;</t>
+        </is>
+      </c>
+      <c r="G6" s="0" t="inlineStr">
+        <is>
+          <t>Instituto de Química de São Carlos  / Universidade de São Paulo</t>
+        </is>
+      </c>
+      <c r="H6" s="0" t="inlineStr">
+        <is>
+          <t>Caroline Ceribeli;</t>
+        </is>
+      </c>
+      <c r="I6" s="0" t="inlineStr">
+        <is>
+          <t>Instituto de Química de São Carlos/ Universidade de São Paulo</t>
+        </is>
+      </c>
+      <c r="J6" s="0" t="inlineStr">
+        <is>
+          <t>Luiz Alberto Colnago;</t>
+        </is>
+      </c>
+      <c r="K6" s="0" t="inlineStr">
+        <is>
+          <t>Empresa Brasileira de Pesquisa Agropecuária</t>
+        </is>
+      </c>
+      <c r="L6" s="0" t="inlineStr">
+        <is>
+          <t>Daniel Cardoso;</t>
+        </is>
+      </c>
+      <c r="M6" s="0" t="inlineStr">
+        <is>
+          <t>Instituto de Química de São Carlos  / Universidade de São Paulo</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="0" t="inlineStr">
         <is>
           <t>137466</t>
@@ -350,8 +640,38 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>Enya Silva de Oliveira;</t>
+        </is>
+      </c>
+      <c r="E7" s="0" t="inlineStr">
+        <is>
+          <t>Institute of Chemistry/Federal University of Goiás</t>
+        </is>
+      </c>
+      <c r="F7" s="0" t="inlineStr">
+        <is>
+          <t>Luciano Morais Lião;</t>
+        </is>
+      </c>
+      <c r="G7" s="0" t="inlineStr">
+        <is>
+          <t>Institute of Chemistry/Federal University of Goiás</t>
+        </is>
+      </c>
+      <c r="H7" s="0" t="inlineStr">
+        <is>
+          <t>Gerlon de Almeida Ribeiro Oliveira;</t>
+        </is>
+      </c>
+      <c r="I7" s="0" t="inlineStr">
+        <is>
+          <t>Institute of Chemistry/Federal University of Goiás</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="0" t="inlineStr">
         <is>
           <t>137468</t>
@@ -367,8 +687,28 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>Amanda de Souza;</t>
+        </is>
+      </c>
+      <c r="E8" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal dos Vales do Jequitinhonha e Mucuri</t>
+        </is>
+      </c>
+      <c r="F8" s="0" t="inlineStr">
+        <is>
+          <t>Rodrigo Verly;</t>
+        </is>
+      </c>
+      <c r="G8" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal dos Vales do Jequitinhonha e Mucuri</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="0" t="inlineStr">
         <is>
           <t>137469</t>
@@ -384,8 +724,68 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" s="0" t="inlineStr">
+        <is>
+          <t>Daniel Lysak;</t>
+        </is>
+      </c>
+      <c r="E9" s="0" t="inlineStr">
+        <is>
+          <t>Chemistry / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
+      <c r="F9" s="0" t="inlineStr">
+        <is>
+          <t>FLAVIO VINICIUS CRIZOSTOMO  KOCK;</t>
+        </is>
+      </c>
+      <c r="G9" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal de São Carlos</t>
+        </is>
+      </c>
+      <c r="H9" s="0" t="inlineStr">
+        <is>
+          <t>Salvatore Mamone;</t>
+        </is>
+      </c>
+      <c r="I9" s="0" t="inlineStr">
+        <is>
+          <t>Biophysical Chemistry / Max Planck Institute / Max Planck Institute for Biophysical Chemistry</t>
+        </is>
+      </c>
+      <c r="J9" s="0" t="inlineStr">
+        <is>
+          <t>Stefan Glöggler;</t>
+        </is>
+      </c>
+      <c r="K9" s="0" t="inlineStr">
+        <is>
+          <t>Biophysical Chemistry / Max Planck Institute / Max Planck Institute for Biophysical Chemistry</t>
+        </is>
+      </c>
+      <c r="L9" s="0" t="inlineStr">
+        <is>
+          <t>Ronald Soong;</t>
+        </is>
+      </c>
+      <c r="M9" s="0" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
+      <c r="N9" s="0" t="inlineStr">
+        <is>
+          <t>Andre Simpson;</t>
+        </is>
+      </c>
+      <c r="O9" s="0" t="inlineStr">
+        <is>
+          <t>University of Toronto</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="0" t="inlineStr">
         <is>
           <t>137470</t>
@@ -401,8 +801,38 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" s="0" t="inlineStr">
+        <is>
+          <t>Kennedy  Daniel  de Carvalho Santos;</t>
+        </is>
+      </c>
+      <c r="E10" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
+        </is>
+      </c>
+      <c r="F10" s="0" t="inlineStr">
+        <is>
+          <t>Guilherme Dal Poggetto;</t>
+        </is>
+      </c>
+      <c r="G10" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
+        </is>
+      </c>
+      <c r="H10" s="0" t="inlineStr">
+        <is>
+          <t>Cláudio Francisco Tormena;</t>
+        </is>
+      </c>
+      <c r="I10" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="0" t="inlineStr">
         <is>
           <t>137471</t>
@@ -418,8 +848,58 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" s="0" t="inlineStr">
+        <is>
+          <t>Gustavo  Solcia;</t>
+        </is>
+      </c>
+      <c r="E11" s="0" t="inlineStr">
+        <is>
+          <t>Universidade de São Paulo</t>
+        </is>
+      </c>
+      <c r="F11" s="0" t="inlineStr">
+        <is>
+          <t>Caio de Jesus Oliveira;</t>
+        </is>
+      </c>
+      <c r="G11" s="0" t="inlineStr">
+        <is>
+          <t>Universidade de São Paulo</t>
+        </is>
+      </c>
+      <c r="H11" s="0" t="inlineStr">
+        <is>
+          <t>Rafael Henrique Ferreira da Silva;</t>
+        </is>
+      </c>
+      <c r="I11" s="0" t="inlineStr">
+        <is>
+          <t>Universidade de São Paulo</t>
+        </is>
+      </c>
+      <c r="J11" s="0" t="inlineStr">
+        <is>
+          <t>Felipe Ferraz Derrico;</t>
+        </is>
+      </c>
+      <c r="K11" s="0" t="inlineStr">
+        <is>
+          <t>Universidade de São Paulo</t>
+        </is>
+      </c>
+      <c r="L11" s="0" t="inlineStr">
+        <is>
+          <t>Fernando Fernandes Paiva;</t>
+        </is>
+      </c>
+      <c r="M11" s="0" t="inlineStr">
+        <is>
+          <t>Instituto de Física de São Carlos</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="0" t="inlineStr">
         <is>
           <t>137472</t>
@@ -435,8 +915,48 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" s="0" t="inlineStr">
+        <is>
+          <t>Pedro Henrique Soares Cardoso;</t>
+        </is>
+      </c>
+      <c r="E12" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal de Goiás</t>
+        </is>
+      </c>
+      <c r="F12" s="0" t="inlineStr">
+        <is>
+          <t>Luciano Morais Lião;</t>
+        </is>
+      </c>
+      <c r="G12" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal de Goiás</t>
+        </is>
+      </c>
+      <c r="H12" s="0" t="inlineStr">
+        <is>
+          <t>Enya Silva de Oliveira;</t>
+        </is>
+      </c>
+      <c r="I12" s="0" t="inlineStr">
+        <is>
+          <t>Institute of Chemistry/Federal University of Goiás</t>
+        </is>
+      </c>
+      <c r="J12" s="0" t="inlineStr">
+        <is>
+          <t>Gerlon de Almeida Ribeiro Oliveira;</t>
+        </is>
+      </c>
+      <c r="K12" s="0" t="inlineStr">
+        <is>
+          <t>Instituto de Química / Universidade Federal de Goiás</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="0" t="inlineStr">
         <is>
           <t>137473</t>
@@ -452,8 +972,38 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" s="0" t="inlineStr">
+        <is>
+          <t>Marília Vilela Salvador;</t>
+        </is>
+      </c>
+      <c r="E13" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Rio Grande do Sul</t>
+        </is>
+      </c>
+      <c r="F13" s="0" t="inlineStr">
+        <is>
+          <t>Tiago  Venâncio;</t>
+        </is>
+      </c>
+      <c r="G13" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal de São Carlos</t>
+        </is>
+      </c>
+      <c r="H13" s="0" t="inlineStr">
+        <is>
+          <t>Francisco Paulo dos Santos;</t>
+        </is>
+      </c>
+      <c r="I13" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Rio Grande do Sul</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" s="0" t="inlineStr">
         <is>
           <t>137474</t>
@@ -469,8 +1019,98 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" s="0" t="inlineStr">
+        <is>
+          <t>Monica Bastawrous;</t>
+        </is>
+      </c>
+      <c r="E14" s="0" t="inlineStr">
+        <is>
+          <t>University of Toronto</t>
+        </is>
+      </c>
+      <c r="F14" s="0" t="inlineStr">
+        <is>
+          <t>Rajshree Ghosh Biswas;</t>
+        </is>
+      </c>
+      <c r="G14" s="0" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
+      <c r="H14" s="0" t="inlineStr">
+        <is>
+          <t>Ronald Soong;</t>
+        </is>
+      </c>
+      <c r="I14" s="0" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
+      <c r="J14" s="0" t="inlineStr">
+        <is>
+          <t>Sagar Wadhwa;</t>
+        </is>
+      </c>
+      <c r="K14" s="0" t="inlineStr">
+        <is>
+          <t>Institute of Microstructure Technology / Karlsruhe Institute of Technology / Karlsruhe Institute of Technology</t>
+        </is>
+      </c>
+      <c r="L14" s="0" t="inlineStr">
+        <is>
+          <t>Neil Mackinnon;</t>
+        </is>
+      </c>
+      <c r="M14" s="0" t="inlineStr">
+        <is>
+          <t>Institute of Microstructure Technology / Karlsruhe Institute of Technology / Karlsruhe Institute of Technology</t>
+        </is>
+      </c>
+      <c r="N14" s="0" t="inlineStr">
+        <is>
+          <t>Mazin Jouda;</t>
+        </is>
+      </c>
+      <c r="O14" s="0" t="inlineStr">
+        <is>
+          <t>Institute of Microstructure Technology / Karlsruhe Institute of Technology / Karlsruhe Institute of Technology</t>
+        </is>
+      </c>
+      <c r="P14" s="0" t="inlineStr">
+        <is>
+          <t>Dario Mager;</t>
+        </is>
+      </c>
+      <c r="Q14" s="0" t="inlineStr">
+        <is>
+          <t>Institute of Microstructure Technology / Karlsruhe Institute of Technology / Karlsruhe Institute of Technology</t>
+        </is>
+      </c>
+      <c r="R14" s="0" t="inlineStr">
+        <is>
+          <t>Jan Korvink;</t>
+        </is>
+      </c>
+      <c r="S14" s="0" t="inlineStr">
+        <is>
+          <t>Institute of Microstructure Technology / Karlsruhe Institute of Technology / Karlsruhe Institute of Technology</t>
+        </is>
+      </c>
+      <c r="T14" s="0" t="inlineStr">
+        <is>
+          <t>Andre Simpson;</t>
+        </is>
+      </c>
+      <c r="U14" s="0" t="inlineStr">
+        <is>
+          <t>University of Toronto</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" s="0" t="inlineStr">
         <is>
           <t>137476</t>
@@ -486,8 +1126,88 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" s="0" t="inlineStr">
+        <is>
+          <t>Yara Rocha;</t>
+        </is>
+      </c>
+      <c r="E15" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
+        </is>
+      </c>
+      <c r="F15" s="0" t="inlineStr">
+        <is>
+          <t>Victor U. Antunes;</t>
+        </is>
+      </c>
+      <c r="G15" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
+        </is>
+      </c>
+      <c r="H15" s="0" t="inlineStr">
+        <is>
+          <t>Yan  Ladeira;</t>
+        </is>
+      </c>
+      <c r="I15" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal de Minas Gerais</t>
+        </is>
+      </c>
+      <c r="J15" s="0" t="inlineStr">
+        <is>
+          <t>Adolfo Henrique de Moraes Silva;</t>
+        </is>
+      </c>
+      <c r="K15" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal de Minas Gerais</t>
+        </is>
+      </c>
+      <c r="L15" s="0" t="inlineStr">
+        <is>
+          <t>Renan Pirolla;</t>
+        </is>
+      </c>
+      <c r="M15" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
+        </is>
+      </c>
+      <c r="N15" s="0" t="inlineStr">
+        <is>
+          <t>Fábio Gozzo;</t>
+        </is>
+      </c>
+      <c r="O15" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
+        </is>
+      </c>
+      <c r="P15" s="0" t="inlineStr">
+        <is>
+          <t>Anthony  Mittermaier;</t>
+        </is>
+      </c>
+      <c r="Q15" s="0" t="inlineStr">
+        <is>
+          <t>Department of Chemistry / McGill University / McGill University</t>
+        </is>
+      </c>
+      <c r="R15" s="0" t="inlineStr">
+        <is>
+          <t>Denize  C. Favaro;</t>
+        </is>
+      </c>
+      <c r="S15" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="0" t="inlineStr">
         <is>
           <t>137477</t>
@@ -503,8 +1223,28 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" s="0" t="inlineStr">
+        <is>
+          <t>Cassia  Chiari;</t>
+        </is>
+      </c>
+      <c r="E16" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
+        </is>
+      </c>
+      <c r="F16" s="0" t="inlineStr">
+        <is>
+          <t>Cláudio Francisco Tormena;</t>
+        </is>
+      </c>
+      <c r="G16" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="0" t="inlineStr">
         <is>
           <t>137478</t>
@@ -520,8 +1260,38 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>Flávio Bueno dos Santos;</t>
+        </is>
+      </c>
+      <c r="E17" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal de Ouro Preto</t>
+        </is>
+      </c>
+      <c r="F17" s="0" t="inlineStr">
+        <is>
+          <t>Marcus Cardoso;</t>
+        </is>
+      </c>
+      <c r="G17" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal de Ouro Preto</t>
+        </is>
+      </c>
+      <c r="H17" s="0" t="inlineStr">
+        <is>
+          <t>Jose Rivera;</t>
+        </is>
+      </c>
+      <c r="I17" s="0" t="inlineStr">
+        <is>
+          <t>Universidade de São Paulo</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="0" t="inlineStr">
         <is>
           <t>137479</t>
@@ -537,8 +1307,68 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>Priscila  Rubim;</t>
+        </is>
+      </c>
+      <c r="E18" s="0" t="inlineStr">
+        <is>
+          <t>Instituto Militar de Engenharia</t>
+        </is>
+      </c>
+      <c r="F18" s="0" t="inlineStr">
+        <is>
+          <t>Mychelle Monteiro;</t>
+        </is>
+      </c>
+      <c r="G18" s="0" t="inlineStr">
+        <is>
+          <t>INCQS / Fundação Oswaldo Cruz</t>
+        </is>
+      </c>
+      <c r="H18" s="0" t="inlineStr">
+        <is>
+          <t>Filipe Soares Quirino da Silva;</t>
+        </is>
+      </c>
+      <c r="I18" s="0" t="inlineStr">
+        <is>
+          <t>INCQS/Fiocruz</t>
+        </is>
+      </c>
+      <c r="J18" s="0" t="inlineStr">
+        <is>
+          <t>Tanos Celmar Costa França;</t>
+        </is>
+      </c>
+      <c r="K18" s="0" t="inlineStr">
+        <is>
+          <t>Instituto Militar de Engenharia</t>
+        </is>
+      </c>
+      <c r="L18" s="0" t="inlineStr">
+        <is>
+          <t>Joyce Sobreiro Francisco Diz de Almeida;</t>
+        </is>
+      </c>
+      <c r="M18" s="0" t="inlineStr">
+        <is>
+          <t>Instituto Militar de Engenharia</t>
+        </is>
+      </c>
+      <c r="N18" s="0" t="inlineStr">
+        <is>
+          <t>Jochen  Junker;</t>
+        </is>
+      </c>
+      <c r="O18" s="0" t="inlineStr">
+        <is>
+          <t>CDTS / Presidência / Fundação Oswaldo Cruz</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="0" t="inlineStr">
         <is>
           <t>137480</t>
@@ -554,8 +1384,28 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" s="0" t="inlineStr">
+        <is>
+          <t>Laiza  Bruzadelle Loureiro;</t>
+        </is>
+      </c>
+      <c r="E19" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
+        </is>
+      </c>
+      <c r="F19" s="0" t="inlineStr">
+        <is>
+          <t>Cláudio Francisco Tormena;</t>
+        </is>
+      </c>
+      <c r="G19" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Estadual de Campinas</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
       <c r="A20" s="0" t="inlineStr">
         <is>
           <t>137486</t>
@@ -571,8 +1421,48 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20" s="0" t="inlineStr">
+        <is>
+          <t>Vinícius  Silva Pinto;</t>
+        </is>
+      </c>
+      <c r="E20" s="0" t="inlineStr">
+        <is>
+          <t>Federal Institute Goiano</t>
+        </is>
+      </c>
+      <c r="F20" s="0" t="inlineStr">
+        <is>
+          <t>Christian Dias Gomides;</t>
+        </is>
+      </c>
+      <c r="G20" s="0" t="inlineStr">
+        <is>
+          <t>Institute of Chemistry, Federal University of Goias</t>
+        </is>
+      </c>
+      <c r="H20" s="0" t="inlineStr">
+        <is>
+          <t>Igor Flores;</t>
+        </is>
+      </c>
+      <c r="I20" s="0" t="inlineStr">
+        <is>
+          <t>Federal Institute of Goiás</t>
+        </is>
+      </c>
+      <c r="J20" s="0" t="inlineStr">
+        <is>
+          <t>Luciano Morais Lião;</t>
+        </is>
+      </c>
+      <c r="K20" s="0" t="inlineStr">
+        <is>
+          <t>Institute of Chemistry, Federal University of Goias</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
       <c r="A21" s="0" t="inlineStr">
         <is>
           <t>137487</t>
@@ -588,8 +1478,48 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21" s="0" t="inlineStr">
+        <is>
+          <t>José Dias de Souza Filho;</t>
+        </is>
+      </c>
+      <c r="E21" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal de Ouro Preto</t>
+        </is>
+      </c>
+      <c r="F21" s="0" t="inlineStr">
+        <is>
+          <t>Jacqueline Souza;</t>
+        </is>
+      </c>
+      <c r="G21" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal de Ouro Preto</t>
+        </is>
+      </c>
+      <c r="H21" s="0" t="inlineStr">
+        <is>
+          <t>Marta de Lana;</t>
+        </is>
+      </c>
+      <c r="I21" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal de Ouro Preto</t>
+        </is>
+      </c>
+      <c r="J21" s="0" t="inlineStr">
+        <is>
+          <t>Gabriela Roberta Ramos Fernandes;</t>
+        </is>
+      </c>
+      <c r="K21" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal de Ouro Preto</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="0" t="inlineStr">
         <is>
           <t>137555</t>
@@ -605,8 +1535,58 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22" s="0" t="inlineStr">
+        <is>
+          <t>Beatriz Rosa  Penna;</t>
+        </is>
+      </c>
+      <c r="E22" s="0" t="inlineStr">
+        <is>
+          <t>Instituto de Bioquímica Médica, Centro Nacional de Ressonância Magnética Nuclear Jiri Jonas, Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
+      <c r="F22" s="0" t="inlineStr">
+        <is>
+          <t>Thamires Moreira;</t>
+        </is>
+      </c>
+      <c r="G22" s="0" t="inlineStr">
+        <is>
+          <t>Departamento de Bioquímica, Instituto de Química, Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
+      <c r="H22" s="0" t="inlineStr">
+        <is>
+          <t>Danielle Maria  Perpétua de Oliveira Santos;</t>
+        </is>
+      </c>
+      <c r="I22" s="0" t="inlineStr">
+        <is>
+          <t>Departamento de Bioquímica, Instituto de Química, Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
+      <c r="J22" s="0" t="inlineStr">
+        <is>
+          <t>Cristiane Dinis Ano Bom;</t>
+        </is>
+      </c>
+      <c r="K22" s="0" t="inlineStr">
+        <is>
+          <t>Departamento de Bioquímica, Instituto de Química, Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
+      <c r="L22" s="0" t="inlineStr">
+        <is>
+          <t>Ana Paula Valente;</t>
+        </is>
+      </c>
+      <c r="M22" s="0" t="inlineStr">
+        <is>
+          <t>Instituto de Bioquímica Médica, Centro Nacional de Ressonância Magnética Nuclear Jiri Jonas, Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23" s="0" t="inlineStr">
         <is>
           <t>137556</t>
@@ -622,8 +1602,78 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23" s="0" t="inlineStr">
+        <is>
+          <t>Julie Lopes;</t>
+        </is>
+      </c>
+      <c r="E23" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
+      <c r="F23" s="0" t="inlineStr">
+        <is>
+          <t>Beatriz Rosa  Penna;</t>
+        </is>
+      </c>
+      <c r="G23" s="0" t="inlineStr">
+        <is>
+          <t>Instituto de Bioquímica Médica, Centro Nacional de Ressonância Magnética Nuclear Jiri Jonas, Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
+      <c r="H23" s="0" t="inlineStr">
+        <is>
+          <t>Ana Paula Valente;</t>
+        </is>
+      </c>
+      <c r="I23" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
+      <c r="J23" s="0" t="inlineStr">
+        <is>
+          <t>Leonardo  Bartkevihi;</t>
+        </is>
+      </c>
+      <c r="K23" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
+      <c r="L23" s="0" t="inlineStr">
+        <is>
+          <t>Paulo Antônio de Souza Mourão;</t>
+        </is>
+      </c>
+      <c r="M23" s="0" t="inlineStr">
+        <is>
+          <t>Laboratório de Tecido Conjuntivo / Instituto de Bioquímica Médica / Universidade Federal de Juiz de Fora</t>
+        </is>
+      </c>
+      <c r="N23" s="0" t="inlineStr">
+        <is>
+          <t>Francisco  Felipe  Bezerra;</t>
+        </is>
+      </c>
+      <c r="O23" s="0" t="inlineStr">
+        <is>
+          <t>Departamento de Glicobiologia  / Bioquímica Médica / Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
+      <c r="P23" s="0" t="inlineStr">
+        <is>
+          <t>Adriane Regina Todeschini;</t>
+        </is>
+      </c>
+      <c r="Q23" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
       <c r="A24" s="0" t="inlineStr">
         <is>
           <t>139165</t>
@@ -639,8 +1689,48 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24" s="0" t="inlineStr">
+        <is>
+          <t>Elton Tadeu Montrazi;</t>
+        </is>
+      </c>
+      <c r="E24" s="0" t="inlineStr">
+        <is>
+          <t>Department of Chemical and Biological Physics, Weizmann Institute of Science, Israel</t>
+        </is>
+      </c>
+      <c r="F24" s="0" t="inlineStr">
+        <is>
+          <t>Tatiana Monaretto;</t>
+        </is>
+      </c>
+      <c r="G24" s="0" t="inlineStr">
+        <is>
+          <t>Centre National de La Recherche Scientifique, France</t>
+        </is>
+      </c>
+      <c r="H24" s="0" t="inlineStr">
+        <is>
+          <t>Luiz Alberto Colnago;</t>
+        </is>
+      </c>
+      <c r="I24" s="0" t="inlineStr">
+        <is>
+          <t>Embrapa Instrumentation, Brazil</t>
+        </is>
+      </c>
+      <c r="J24" s="0" t="inlineStr">
+        <is>
+          <t>Tito José Bonagamba;</t>
+        </is>
+      </c>
+      <c r="K24" s="0" t="inlineStr">
+        <is>
+          <t>São Carlos Institute of Physics, University of São Paulo, Brazil</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="0" t="inlineStr">
         <is>
           <t>139166</t>
@@ -656,8 +1746,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25" s="0" t="inlineStr">
+        <is>
+          <t>Tatiana Monaretto;</t>
+        </is>
+      </c>
+      <c r="E25" s="0" t="inlineStr">
+        <is>
+          <t>Centre national de la recherche scientifique (CNRS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="0" t="inlineStr">
         <is>
           <t>139167</t>
@@ -673,8 +1773,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="D26" s="0" t="inlineStr">
+        <is>
+          <t>Patrick Giraudeau;</t>
+        </is>
+      </c>
+      <c r="E26" s="0" t="inlineStr">
+        <is>
+          <t>CEISAM / Faculté des Sciences et Techniques / Université de Nantes</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="0" t="inlineStr">
         <is>
           <t>139168</t>
@@ -690,8 +1800,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="D27" s="0" t="inlineStr">
+        <is>
+          <t>Andre Simpson;</t>
+        </is>
+      </c>
+      <c r="E27" s="0" t="inlineStr">
+        <is>
+          <t>University of Toronto</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="0" t="inlineStr">
         <is>
           <t>139169</t>
@@ -707,8 +1827,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="D28" s="0" t="inlineStr">
+        <is>
+          <t>Zeev Wiesman;</t>
+        </is>
+      </c>
+      <c r="E28" s="0" t="inlineStr">
+        <is>
+          <t>LowField</t>
+        </is>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="0" t="inlineStr">
         <is>
           <t>139170</t>
@@ -724,8 +1854,28 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="D29" s="0" t="inlineStr">
+        <is>
+          <t>Flavio Vinicius Crizostomo  Kock;</t>
+        </is>
+      </c>
+      <c r="E29" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal de São Carlos</t>
+        </is>
+      </c>
+      <c r="F29" s="0" t="inlineStr">
+        <is>
+          <t>Tiago Venâncio;</t>
+        </is>
+      </c>
+      <c r="G29" s="0" t="inlineStr">
+        <is>
+          <t>Departamento de Química / Universidade Federal de São Carlos</t>
+        </is>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="0" t="inlineStr">
         <is>
           <t>139172</t>
@@ -741,8 +1891,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="D30" s="0" t="inlineStr">
+        <is>
+          <t>Juan Miguel López del Amo;</t>
+        </is>
+      </c>
+      <c r="E30" s="0" t="inlineStr">
+        <is>
+          <t>NMR  / CIC energigune / CIC energigune</t>
+        </is>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="0" t="inlineStr">
         <is>
           <t>139173</t>
@@ -758,8 +1918,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="D31" s="0" t="inlineStr">
+        <is>
+          <t>Jeffrey Reimer;</t>
+        </is>
+      </c>
+      <c r="E31" s="0" t="inlineStr">
+        <is>
+          <t>Dept Chem and BioM Engr / University of California</t>
+        </is>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="0" t="inlineStr">
         <is>
           <t>139174</t>
@@ -775,8 +1945,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="D32" s="0" t="inlineStr">
+        <is>
+          <t>Daniel Huster;</t>
+        </is>
+      </c>
+      <c r="E32" s="0" t="inlineStr">
+        <is>
+          <t>University of Leipzig</t>
+        </is>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="0" t="inlineStr">
         <is>
           <t>139175</t>
@@ -792,8 +1972,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="34" spans="1:3">
+      <c r="D33" s="0" t="inlineStr">
+        <is>
+          <t>Pau Nolis;</t>
+        </is>
+      </c>
+      <c r="E33" s="0" t="inlineStr">
+        <is>
+          <t>Universitat Autònoma de Barcelona</t>
+        </is>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="0" t="inlineStr">
         <is>
           <t>139176</t>
@@ -809,8 +1999,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="35" spans="1:3">
+      <c r="D34" s="0" t="inlineStr">
+        <is>
+          <t>Josep Saurí;</t>
+        </is>
+      </c>
+      <c r="E34" s="0" t="inlineStr">
+        <is>
+          <t>NMR Research Scientist</t>
+        </is>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="0" t="inlineStr">
         <is>
           <t>139177</t>
@@ -826,8 +2026,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="36" spans="1:3">
+      <c r="D35" s="0" t="inlineStr">
+        <is>
+          <t>Gareth Morris;</t>
+        </is>
+      </c>
+      <c r="E35" s="0" t="inlineStr">
+        <is>
+          <t>The University of Manchester</t>
+        </is>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="0" t="inlineStr">
         <is>
           <t>139178</t>
@@ -843,8 +2053,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="37" spans="1:3">
+      <c r="D36" s="0" t="inlineStr">
+        <is>
+          <t>Antonio Gilberto Ferreira;</t>
+        </is>
+      </c>
+      <c r="E36" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal de São Carlos</t>
+        </is>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="0" t="inlineStr">
         <is>
           <t>139180</t>
@@ -860,8 +2080,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="38" spans="1:3">
+      <c r="D37" s="0" t="inlineStr">
+        <is>
+          <t>Scott Prosser;</t>
+        </is>
+      </c>
+      <c r="E37" s="0" t="inlineStr">
+        <is>
+          <t>University of Toronto</t>
+        </is>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" s="0" t="inlineStr">
         <is>
           <t>139181</t>
@@ -877,8 +2107,38 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="39" spans="1:3">
+      <c r="D38" s="0" t="inlineStr">
+        <is>
+          <t> Jeremy Good;</t>
+        </is>
+      </c>
+      <c r="E38" s="0" t="inlineStr">
+        <is>
+          <t>London, UK / Cryogenic Ltd</t>
+        </is>
+      </c>
+      <c r="F38" s="0" t="inlineStr">
+        <is>
+          <t>Eugeny Kryukov;</t>
+        </is>
+      </c>
+      <c r="G38" s="0" t="inlineStr">
+        <is>
+          <t>Cryogenic Ltd</t>
+        </is>
+      </c>
+      <c r="H38" s="0" t="inlineStr">
+        <is>
+          <t>Dr. Stephen Burgess;</t>
+        </is>
+      </c>
+      <c r="I38" s="0" t="inlineStr">
+        <is>
+          <t>Cryogenic Ltd</t>
+        </is>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="0" t="inlineStr">
         <is>
           <t>139183</t>
@@ -894,8 +2154,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="40" spans="1:3">
+      <c r="D39" s="0" t="inlineStr">
+        <is>
+          <t>Giselle de Araujo Lima e Souza;</t>
+        </is>
+      </c>
+      <c r="E39" s="0" t="inlineStr">
+        <is>
+          <t>Department of Chemistry, Materials and Chemical Engineering “Giulio Natta” / Politecnico di Milano</t>
+        </is>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="0" t="inlineStr">
         <is>
           <t>139184</t>
@@ -911,8 +2181,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="41" spans="1:3">
+      <c r="D40" s="0" t="inlineStr">
+        <is>
+          <t>Ariel Sarotti;</t>
+        </is>
+      </c>
+      <c r="E40" s="0" t="inlineStr">
+        <is>
+          <t>Chimica / Chimica / Universidad Nacional de Rosario</t>
+        </is>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="0" t="inlineStr">
         <is>
           <t>139185</t>
@@ -928,8 +2208,28 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="D41" s="0" t="inlineStr">
+        <is>
+          <t>Sophia Hayes;</t>
+        </is>
+      </c>
+      <c r="E41" s="0" t="inlineStr">
+        <is>
+          <t>Chemistry / Arts &amp; Sciences / Washington University in St. Louis</t>
+        </is>
+      </c>
+      <c r="F41" s="0" t="inlineStr">
+        <is>
+          <t>He Sun;</t>
+        </is>
+      </c>
+      <c r="G41" s="0" t="inlineStr">
+        <is>
+          <t>Chemistry / Arts &amp; Sciences / Washington University in St. Louis</t>
+        </is>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="0" t="inlineStr">
         <is>
           <t>139186</t>
@@ -945,8 +2245,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="43" spans="1:3">
+      <c r="D42" s="0" t="inlineStr">
+        <is>
+          <t>Jair Freitas;</t>
+        </is>
+      </c>
+      <c r="E42" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Espírito Santo, Brazil</t>
+        </is>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" s="0" t="inlineStr">
         <is>
           <t>139187</t>
@@ -962,8 +2272,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="44" spans="1:3">
+      <c r="D43" s="0" t="inlineStr">
+        <is>
+          <t>Toshikazu Miyoshi;</t>
+        </is>
+      </c>
+      <c r="E43" s="0" t="inlineStr">
+        <is>
+          <t>The University of Akron</t>
+        </is>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="0" t="inlineStr">
         <is>
           <t>139188</t>
@@ -979,8 +2299,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="45" spans="1:3">
+      <c r="D44" s="0" t="inlineStr">
+        <is>
+          <t>Marek Pruski;</t>
+        </is>
+      </c>
+      <c r="E44" s="0" t="inlineStr">
+        <is>
+          <t>Iowa State University</t>
+        </is>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="0" t="inlineStr">
         <is>
           <t>139190</t>
@@ -996,8 +2326,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="D45" s="0" t="inlineStr">
+        <is>
+          <t>Yushan Wei;</t>
+        </is>
+      </c>
+      <c r="E45" s="0" t="inlineStr">
+        <is>
+          <t>Niumag</t>
+        </is>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" s="0" t="inlineStr">
         <is>
           <t>139192</t>
@@ -1013,8 +2353,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="47" spans="1:3">
+      <c r="D46" s="0" t="inlineStr">
+        <is>
+          <t>Juan Araneda;</t>
+        </is>
+      </c>
+      <c r="E46" s="0" t="inlineStr">
+        <is>
+          <t>Nanalysis Corp.</t>
+        </is>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" s="0" t="inlineStr">
         <is>
           <t>139193</t>
@@ -1030,8 +2380,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="D47" s="0" t="inlineStr">
+        <is>
+          <t>Clemens Anklin;</t>
+        </is>
+      </c>
+      <c r="E47" s="0" t="inlineStr">
+        <is>
+          <t>Bruker</t>
+        </is>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" s="0" t="inlineStr">
         <is>
           <t>139194</t>
@@ -1047,8 +2407,38 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="D48" s="0" t="inlineStr">
+        <is>
+          <t>Søren Balling Engelsen;</t>
+        </is>
+      </c>
+      <c r="E48" s="0" t="inlineStr">
+        <is>
+          <t>University of Copenhagen</t>
+        </is>
+      </c>
+      <c r="F48" s="0" t="inlineStr">
+        <is>
+          <t>Bekzod  Khakimov ;</t>
+        </is>
+      </c>
+      <c r="G48" s="0" t="inlineStr">
+        <is>
+          <t>University of Copenhagen</t>
+        </is>
+      </c>
+      <c r="H48" s="0" t="inlineStr">
+        <is>
+          <t>Viola  Aru;</t>
+        </is>
+      </c>
+      <c r="I48" s="0" t="inlineStr">
+        <is>
+          <t>University of Copenhagen</t>
+        </is>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" s="0" t="inlineStr">
         <is>
           <t>139195</t>
@@ -1064,8 +2454,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="D49" s="0" t="inlineStr">
+        <is>
+          <t>Felipe Simoes;</t>
+        </is>
+      </c>
+      <c r="E49" s="0" t="inlineStr">
+        <is>
+          <t>Hélio para Ressonancia Magnética / Hélio para Ressonancia Magnética / Air Products do Brasil Ltda</t>
+        </is>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" s="0" t="inlineStr">
         <is>
           <t>139189</t>
@@ -1081,8 +2481,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="D50" s="0" t="inlineStr">
+        <is>
+          <t>Marcel Lachenmann;</t>
+        </is>
+      </c>
+      <c r="E50" s="0" t="inlineStr">
+        <is>
+          <t>Oxford Instruments</t>
+        </is>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" s="0" t="inlineStr">
         <is>
           <t>139191</t>
@@ -1098,8 +2508,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="52" spans="1:3">
+      <c r="D51" s="0" t="inlineStr">
+        <is>
+          <t>Hector Robert;</t>
+        </is>
+      </c>
+      <c r="E51" s="0" t="inlineStr">
+        <is>
+          <t>Magritek, Inc</t>
+        </is>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" s="0" t="inlineStr">
         <is>
           <t>139179</t>
@@ -1115,8 +2535,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="53" spans="1:3">
+      <c r="D52" s="0" t="inlineStr">
+        <is>
+          <t>Marcus Vinícius Cangussu Cardoso;</t>
+        </is>
+      </c>
+      <c r="E52" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal de Ouro Preto</t>
+        </is>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" s="0" t="inlineStr">
         <is>
           <t>139171</t>
@@ -1132,8 +2562,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="D53" s="0" t="inlineStr">
+        <is>
+          <t>Annick Moing;</t>
+        </is>
+      </c>
+      <c r="E53" s="0" t="inlineStr">
+        <is>
+          <t>INRAE Bordeaux, France</t>
+        </is>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
       <c r="A54" s="0" t="inlineStr">
         <is>
           <t>137467</t>
@@ -1149,8 +2589,58 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="55" spans="1:3">
+      <c r="D54" s="0" t="inlineStr">
+        <is>
+          <t>Igor d'Anciães Almeida Silva;</t>
+        </is>
+      </c>
+      <c r="E54" s="0" t="inlineStr">
+        <is>
+          <t>Universidade de São Paulo</t>
+        </is>
+      </c>
+      <c r="F54" s="0" t="inlineStr">
+        <is>
+          <t>Hellmut Eckert;</t>
+        </is>
+      </c>
+      <c r="G54" s="0" t="inlineStr">
+        <is>
+          <t>Universidade de São Paulo</t>
+        </is>
+      </c>
+      <c r="H54" s="0" t="inlineStr">
+        <is>
+          <t>Ana Candida Martins Rodrigues;</t>
+        </is>
+      </c>
+      <c r="I54" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal de São Carlos</t>
+        </is>
+      </c>
+      <c r="J54" s="0" t="inlineStr">
+        <is>
+          <t>Adraiana Nieto-Munoz;</t>
+        </is>
+      </c>
+      <c r="K54" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal de São Carlos</t>
+        </is>
+      </c>
+      <c r="L54" s="0" t="inlineStr">
+        <is>
+          <t>Vinicius Zallocco;</t>
+        </is>
+      </c>
+      <c r="M54" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal de São Carlos</t>
+        </is>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55" s="0" t="inlineStr">
         <is>
           <t>139182</t>
@@ -1166,8 +2656,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="56" spans="1:3">
+      <c r="D55" s="0" t="inlineStr">
+        <is>
+          <t>Esteban Anoardo;</t>
+        </is>
+      </c>
+      <c r="E55" s="0" t="inlineStr">
+        <is>
+          <t>Laboratorio de Relaxometría y Técnicas Especiales (LaRTE). / Instituto de Física Enrique Gaviola, CONICET. Córdoba, Argentina. / FaMAF - Universidad Nacional de Córdoba. Córdoba, Argentina.</t>
+        </is>
+      </c>
+    </row>
+    <row r="56" spans="1:39">
       <c r="A56" s="0" t="inlineStr">
         <is>
           <t>137461</t>
@@ -1183,8 +2683,188 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="57" spans="1:3">
+      <c r="D56" s="0" t="inlineStr">
+        <is>
+          <t>Amy Jenne;</t>
+        </is>
+      </c>
+      <c r="E56" s="0" t="inlineStr">
+        <is>
+          <t>Chemistry / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
+      <c r="F56" s="0" t="inlineStr">
+        <is>
+          <t>Sebastian Von Der Ecken;</t>
+        </is>
+      </c>
+      <c r="G56" s="0" t="inlineStr">
+        <is>
+          <t>University of Toronto</t>
+        </is>
+      </c>
+      <c r="H56" s="0" t="inlineStr">
+        <is>
+          <t>Vincent Moxley-Paquette;</t>
+        </is>
+      </c>
+      <c r="I56" s="0" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
+      <c r="J56" s="0" t="inlineStr">
+        <is>
+          <t>Ian Swyer;</t>
+        </is>
+      </c>
+      <c r="K56" s="0" t="inlineStr">
+        <is>
+          <t>University of Toronto</t>
+        </is>
+      </c>
+      <c r="L56" s="0" t="inlineStr">
+        <is>
+          <t>Ronald Soong;</t>
+        </is>
+      </c>
+      <c r="M56" s="0" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
+      <c r="N56" s="0" t="inlineStr">
+        <is>
+          <t>Monica Bastawrous;</t>
+        </is>
+      </c>
+      <c r="O56" s="0" t="inlineStr">
+        <is>
+          <t>University of Toronto</t>
+        </is>
+      </c>
+      <c r="P56" s="0" t="inlineStr">
+        <is>
+          <t>Falko Busse;</t>
+        </is>
+      </c>
+      <c r="Q56" s="0" t="inlineStr">
+        <is>
+          <t>Bruker</t>
+        </is>
+      </c>
+      <c r="R56" s="0" t="inlineStr">
+        <is>
+          <t>Wolfgang Bermel;</t>
+        </is>
+      </c>
+      <c r="S56" s="0" t="inlineStr">
+        <is>
+          <t>Biospin GmbH / BRUKER</t>
+        </is>
+      </c>
+      <c r="T56" s="0" t="inlineStr">
+        <is>
+          <t>Daniel Schmidig;</t>
+        </is>
+      </c>
+      <c r="U56" s="0" t="inlineStr">
+        <is>
+          <t>Biospin AG / BRUKER</t>
+        </is>
+      </c>
+      <c r="V56" s="0" t="inlineStr">
+        <is>
+          <t>Till Kuehn;</t>
+        </is>
+      </c>
+      <c r="W56" s="0" t="inlineStr">
+        <is>
+          <t>Biospin AG / BRUKER</t>
+        </is>
+      </c>
+      <c r="X56" s="0" t="inlineStr">
+        <is>
+          <t>Rainer Kuemmerle;</t>
+        </is>
+      </c>
+      <c r="Y56" s="0" t="inlineStr">
+        <is>
+          <t>Biospin AG / BRUKER</t>
+        </is>
+      </c>
+      <c r="Z56" s="0" t="inlineStr">
+        <is>
+          <t>Danijela Al Adwan-Stojilkovic;</t>
+        </is>
+      </c>
+      <c r="AA56" s="0" t="inlineStr">
+        <is>
+          <t>Biospin AG / BRUKER</t>
+        </is>
+      </c>
+      <c r="AB56" s="0" t="inlineStr">
+        <is>
+          <t>Stephan Graf;</t>
+        </is>
+      </c>
+      <c r="AC56" s="0" t="inlineStr">
+        <is>
+          <t>Biospin AG / BRUKER</t>
+        </is>
+      </c>
+      <c r="AD56" s="0" t="inlineStr">
+        <is>
+          <t>Thomas Frei;</t>
+        </is>
+      </c>
+      <c r="AE56" s="0" t="inlineStr">
+        <is>
+          <t>Biospin AG / BRUKER</t>
+        </is>
+      </c>
+      <c r="AF56" s="0" t="inlineStr">
+        <is>
+          <t>Martine Monette;</t>
+        </is>
+      </c>
+      <c r="AG56" s="0" t="inlineStr">
+        <is>
+          <t>Canada Ltd / BRUKER</t>
+        </is>
+      </c>
+      <c r="AH56" s="0" t="inlineStr">
+        <is>
+          <t>Henry Stronks;</t>
+        </is>
+      </c>
+      <c r="AI56" s="0" t="inlineStr">
+        <is>
+          <t>Canada Ltd / BRUKER</t>
+        </is>
+      </c>
+      <c r="AJ56" s="0" t="inlineStr">
+        <is>
+          <t>Aaron Wheeler;</t>
+        </is>
+      </c>
+      <c r="AK56" s="0" t="inlineStr">
+        <is>
+          <t>University of Toronto</t>
+        </is>
+      </c>
+      <c r="AL56" s="0" t="inlineStr">
+        <is>
+          <t>Andre Simpson;</t>
+        </is>
+      </c>
+      <c r="AM56" s="0" t="inlineStr">
+        <is>
+          <t>University of Toronto</t>
+        </is>
+      </c>
+    </row>
+    <row r="57" spans="1:29">
       <c r="A57" s="0" t="inlineStr">
         <is>
           <t>137462</t>
@@ -1200,8 +2880,138 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="58" spans="1:3">
+      <c r="D57" s="0" t="inlineStr">
+        <is>
+          <t>Rajshree Ghosh Biswas;</t>
+        </is>
+      </c>
+      <c r="E57" s="0" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
+      <c r="F57" s="0" t="inlineStr">
+        <is>
+          <t>Ronald Soong;</t>
+        </is>
+      </c>
+      <c r="G57" s="0" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
+      <c r="H57" s="0" t="inlineStr">
+        <is>
+          <t>Paris Ning;</t>
+        </is>
+      </c>
+      <c r="I57" s="0" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
+      <c r="J57" s="0" t="inlineStr">
+        <is>
+          <t>Daniel Lane;</t>
+        </is>
+      </c>
+      <c r="K57" s="0" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
+      <c r="L57" s="0" t="inlineStr">
+        <is>
+          <t>Daniel Schmidig;</t>
+        </is>
+      </c>
+      <c r="M57" s="0" t="inlineStr">
+        <is>
+          <t>Biospin AG / Bruker</t>
+        </is>
+      </c>
+      <c r="N57" s="0" t="inlineStr">
+        <is>
+          <t>Peter de Castro;</t>
+        </is>
+      </c>
+      <c r="O57" s="0" t="inlineStr">
+        <is>
+          <t>Biospin AG / Bruker</t>
+        </is>
+      </c>
+      <c r="P57" s="0" t="inlineStr">
+        <is>
+          <t>Stephan Graf;</t>
+        </is>
+      </c>
+      <c r="Q57" s="0" t="inlineStr">
+        <is>
+          <t>Biospin AG / Bruker</t>
+        </is>
+      </c>
+      <c r="R57" s="0" t="inlineStr">
+        <is>
+          <t>Sebastian Wegner;</t>
+        </is>
+      </c>
+      <c r="S57" s="0" t="inlineStr">
+        <is>
+          <t>Bruker Biospin GmbH / Bruker</t>
+        </is>
+      </c>
+      <c r="T57" s="0" t="inlineStr">
+        <is>
+          <t>Falko Busse;</t>
+        </is>
+      </c>
+      <c r="U57" s="0" t="inlineStr">
+        <is>
+          <t>Bruker Biospin GmbH / Bruker</t>
+        </is>
+      </c>
+      <c r="V57" s="0" t="inlineStr">
+        <is>
+          <t>Jochem Struppe;</t>
+        </is>
+      </c>
+      <c r="W57" s="0" t="inlineStr">
+        <is>
+          <t>Bruker BioSpin</t>
+        </is>
+      </c>
+      <c r="X57" s="0" t="inlineStr">
+        <is>
+          <t>Michael  Fey;</t>
+        </is>
+      </c>
+      <c r="Y57" s="0" t="inlineStr">
+        <is>
+          <t>Bruker</t>
+        </is>
+      </c>
+      <c r="Z57" s="0" t="inlineStr">
+        <is>
+          <t>Myrna Simpson;</t>
+        </is>
+      </c>
+      <c r="AA57" s="0" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
+      <c r="AB57" s="0" t="inlineStr">
+        <is>
+          <t>Andre Simpson;</t>
+        </is>
+      </c>
+      <c r="AC57" s="0" t="inlineStr">
+        <is>
+          <t>Department of Physical and Environmental Science / Scarborough Campus / University of Toronto</t>
+        </is>
+      </c>
+    </row>
+    <row r="58" spans="1:17">
       <c r="A58" s="0" t="inlineStr">
         <is>
           <t>137475</t>
@@ -1217,8 +3027,73 @@
           <t>Poster Presentation</t>
         </is>
       </c>
-    </row>
-    <row r="59" spans="1:3">
+      <c r="D58" s="0" t="inlineStr">
+        <is>
+          <t>VANESSA BEZERRA DE OLIVEIRA LEITE;</t>
+        </is>
+      </c>
+      <c r="E58" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Estado do Rio de Janeiro</t>
+        </is>
+      </c>
+      <c r="F58" s="0" t="inlineStr">
+        <is>
+          <t>Talita Stelling De Araujo;</t>
+        </is>
+      </c>
+      <c r="G58" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
+      <c r="H58" s="0" t="inlineStr">
+        <is>
+          <t>Rafael Alves de Andrade;</t>
+        </is>
+      </c>
+      <c r="I58" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
+      <c r="J58" s="0" t="inlineStr">
+        <is>
+          <t> ;</t>
+        </is>
+      </c>
+      <c r="L58" s="0" t="inlineStr">
+        <is>
+          <t>Fabio C. L. Almeida;</t>
+        </is>
+      </c>
+      <c r="M58" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
+      <c r="N58" s="0" t="inlineStr">
+        <is>
+          <t>Marcius da Silva Almeida;</t>
+        </is>
+      </c>
+      <c r="O58" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
+      <c r="P58" s="0" t="inlineStr">
+        <is>
+          <t>Claudia Jorge do Nascimento;</t>
+        </is>
+      </c>
+      <c r="Q58" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Estado do Rio de Janeiro</t>
+        </is>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" s="0" t="inlineStr">
         <is>
           <t>139532</t>
@@ -1234,8 +3109,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="60" spans="1:3">
+      <c r="D59" s="0" t="inlineStr">
+        <is>
+          <t>Fabio Ceneviva  Lacerda Almeida;</t>
+        </is>
+      </c>
+      <c r="E59" s="0" t="inlineStr">
+        <is>
+          <t>Universidade Federal do Rio de Janeiro</t>
+        </is>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" s="0" t="inlineStr">
         <is>
           <t>139533</t>
@@ -1251,8 +3136,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="61" spans="1:3">
+      <c r="D60" s="0" t="inlineStr">
+        <is>
+          <t>Clemens  Anklin;</t>
+        </is>
+      </c>
+      <c r="E60" s="0" t="inlineStr">
+        <is>
+          <t>NMR Applicaitons / Bruker Biospin</t>
+        </is>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61" s="0" t="inlineStr">
         <is>
           <t>139534</t>
@@ -1268,8 +3163,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="62" spans="1:3">
+      <c r="D61" s="0" t="inlineStr">
+        <is>
+          <t>Julien Orts;</t>
+        </is>
+      </c>
+      <c r="E61" s="0" t="inlineStr">
+        <is>
+          <t>Department of Pharmaceutical Sciences / Faculty of Life Sciences / University of Vienna</t>
+        </is>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62" s="0" t="inlineStr">
         <is>
           <t>139531</t>
@@ -1285,8 +3190,18 @@
           <t>Invited Lecturer</t>
         </is>
       </c>
-    </row>
-    <row r="63" spans="1:3">
+      <c r="D62" s="0" t="inlineStr">
+        <is>
+          <t>Donald Bouchard;</t>
+        </is>
+      </c>
+      <c r="E62" s="0" t="inlineStr">
+        <is>
+          <t>Alegre Science Inc</t>
+        </is>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
       <c r="A63" s="0" t="inlineStr">
         <is>
           <t>137463</t>
@@ -1300,6 +3215,56 @@
       <c r="C63" s="0" t="inlineStr">
         <is>
           <t>Poster Presentation</t>
+        </is>
+      </c>
+      <c r="D63" s="0" t="inlineStr">
+        <is>
+          <t>Giselle de Araujo Lima e Souza;</t>
+        </is>
+      </c>
+      <c r="E63" s="0" t="inlineStr">
+        <is>
+          <t>Department of Chemistry, Materials and Chemical Engineering “Giulio Natta” / Politecnico di Milano</t>
+        </is>
+      </c>
+      <c r="F63" s="0" t="inlineStr">
+        <is>
+          <t>Maria Enrica Di Pietro;</t>
+        </is>
+      </c>
+      <c r="G63" s="0" t="inlineStr">
+        <is>
+          <t>Department of Chemistry, Materials and Chemical Engineering “Giulio Natta” / Politecnico di Milano</t>
+        </is>
+      </c>
+      <c r="H63" s="0" t="inlineStr">
+        <is>
+          <t>Giovanni Battista Appetecchi;</t>
+        </is>
+      </c>
+      <c r="I63" s="0" t="inlineStr">
+        <is>
+          <t>Department for Sustainability (SSPT) / Italian National Agency for New Technologies, Energy and Sustainable Economic Development / ENEA</t>
+        </is>
+      </c>
+      <c r="J63" s="0" t="inlineStr">
+        <is>
+          <t>Patricia Fazzio Martinez;</t>
+        </is>
+      </c>
+      <c r="K63" s="0" t="inlineStr">
+        <is>
+          <t>School of Chemical Engineering/ University of Campinas/ Campinas/ Brazil</t>
+        </is>
+      </c>
+      <c r="L63" s="0" t="inlineStr">
+        <is>
+          <t>Andrea Mele;</t>
+        </is>
+      </c>
+      <c r="M63" s="0" t="inlineStr">
+        <is>
+          <t>Department of Chemistry, Materials and Chemical Engineering “Giulio Natta” / Politecnico di Milano</t>
         </is>
       </c>
     </row>

</xml_diff>